<commit_message>
Fix color for day 4
</commit_message>
<xml_diff>
--- a/Day4.xlsx
+++ b/Day4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Personal\AOC2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47057D46-AB5F-4CAB-9D8B-27A4E83508B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA1A4F4-3F0B-413B-A70C-9D43D22C9D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{910A664D-2432-4BF9-9131-288E478D4FCD}"/>
   </bookViews>
@@ -1590,18 +1590,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1609,6 +1597,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2026,7 +2026,7 @@
         <f ca="1">IF(LEN(W1)&gt;0, SUM(O1:S5), "")</f>
         <v>919</v>
       </c>
-      <c r="Y1" s="3">
+      <c r="Y1" s="5">
         <f ca="1">IF(LEN(W1)&gt;0, V1*X1, "")</f>
         <v>45031</v>
       </c>
@@ -2101,7 +2101,7 @@
         <f ca="1">IF(LEN(W2)&gt;0, SUM(O7:S11), "")</f>
         <v>321</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Y2" s="4">
         <f ca="1">IF(LEN(W2)&gt;0, V2*X2, "")</f>
         <v>2568</v>
       </c>
@@ -19666,9 +19666,9 @@
     <col min="11" max="15" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="3" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="3" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="3" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="6.140625" bestFit="1" customWidth="1"/>
@@ -19750,7 +19750,7 @@
         <f ca="1">IF(LEN(AD1)&gt;0, SUM(INDIRECT(ADDRESS(AD1-5,Y3)&amp;":"&amp;ADDRESS(AD1-1,Y4))), "")</f>
         <v>919</v>
       </c>
-      <c r="AF1" s="3">
+      <c r="AF1" s="5">
         <f ca="1">IF(LEN(AD1)&gt;0, AC1*AE1, "")</f>
         <v>45031</v>
       </c>
@@ -19841,7 +19841,7 @@
         <f t="array" aca="1" ref="AE2" ca="1">IF(LEN(AD2)&gt;0, SUM(INDIRECT(ADDRESS(AD2-5,Y5)&amp;":"&amp;ADDRESS(AD2-1,Y6)))-INDIRECT(ADDRESS(AB2+1, Y2)), "")</f>
         <v>321</v>
       </c>
-      <c r="AF2" s="6">
+      <c r="AF2" s="4">
         <f ca="1">IF(LEN(AD2)&gt;0, AC2*AE2, "")</f>
         <v>2568</v>
       </c>
@@ -20804,7 +20804,7 @@
         <f ca="1"/>
         <v>49</v>
       </c>
-      <c r="T17" s="4" t="s">
+      <c r="T17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="U17">
@@ -24914,7 +24914,7 @@
       <c r="U86">
         <v>92</v>
       </c>
-      <c r="V86" s="5" t="s">
+      <c r="V86" s="3" t="s">
         <v>0</v>
       </c>
       <c r="W86">

</xml_diff>